<commit_message>
Update altus instance types, spark sizing
</commit_message>
<xml_diff>
--- a/asystem-adoc/src/site/resources/altus_spark_sizing.xlsx
+++ b/asystem-adoc/src/site/resources/altus_spark_sizing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graham/_/dev/graham/asystem/asystem-adoc/src/site/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955D1DE8-7CBD-2045-8722-CEC3F0603470}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE14DC8-B29A-294D-A49C-1BC62494D8B8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5060" yWindow="2900" windowWidth="43300" windowHeight="20200" xr2:uid="{342B7839-8DF3-8649-8032-CC038C3B89CC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>export CLUSTER_INSTANCE_TYPE=c4.xlarge</t>
   </si>
@@ -79,12 +79,18 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>export SPARK_EXEC_MEMORY=1400m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -250,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -297,49 +303,55 @@
     <xf numFmtId="45" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="45" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -361,6 +373,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -677,21 +713,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97B9F99-D795-2747-B80E-3F5C45A90888}">
-  <dimension ref="B1:K17"/>
+  <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="4.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="38.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="4" customWidth="1"/>
-    <col min="4" max="11" width="19" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="4"/>
+    <col min="3" max="3" width="10" style="4" customWidth="1"/>
+    <col min="4" max="12" width="19.5" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="5" t="s">
@@ -718,12 +756,15 @@
       <c r="K2" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="36" t="s">
+      <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="10">
@@ -748,13 +789,17 @@
         <v>-1</v>
       </c>
       <c r="K3" s="10">
-        <f t="shared" ref="K3:K17" si="0">SUM(D3:J3)</f>
+        <f>SUM(D3:J3)</f>
         <v>-0.97833333333333328</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="40">
+        <f>IF(K3&lt;0,0,ROUND(K3,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="9"/>
-      <c r="C4" s="37"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
       <c r="F4" s="10"/>
@@ -763,15 +808,19 @@
       <c r="I4" s="12"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+        <f>SUM(D4:J4)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="40">
+        <f t="shared" ref="L4:L17" si="0">IF(K4&lt;0,0,ROUND(K4,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="10"/>
       <c r="E5" s="11"/>
       <c r="F5" s="10"/>
@@ -780,15 +829,19 @@
       <c r="I5" s="12"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10">
+        <f>SUM(D5:J5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="10"/>
@@ -797,13 +850,17 @@
       <c r="I6" s="12"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10">
+        <f>SUM(D6:J6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
-        <v>6</v>
+    <row r="7" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="47" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
@@ -837,280 +894,324 @@
         <v>-1</v>
       </c>
       <c r="K7" s="13">
+        <f>SUM(D7:J7)</f>
+        <v>-0.97833333333333328</v>
+      </c>
+      <c r="L7" s="41">
         <f t="shared" si="0"/>
-        <v>-0.97833333333333328</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>3.1365740740740742E-3</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="18">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <v>5.7060185185185191E-3</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="18">
         <v>7.291666666666667E-4</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="16">
         <v>1.6087962962962963E-3</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="16">
+        <f>SUM(D8:J8)</f>
+        <v>2.0798611111111108E-2</v>
+      </c>
+      <c r="L8" s="42">
         <f t="shared" si="0"/>
-        <v>2.0798611111111108E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="16"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="31"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="16">
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>1.2847222222222223E-3</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="16">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="18">
         <v>8.1018518518518516E-4</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="16">
         <v>6.076388888888889E-3</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="18">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="16">
         <v>1.5162037037037036E-3</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="16">
+        <f>SUM(D9:J9)</f>
+        <v>2.1111111111111112E-2</v>
+      </c>
+      <c r="L9" s="42">
         <f t="shared" si="0"/>
-        <v>2.1111111111111112E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17">
+      <c r="C10" s="36"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16">
+        <f>SUM(D10:J10)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+    <row r="11" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17">
+      <c r="C11" s="37"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16">
+        <f>SUM(D11:J11)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+    <row r="12" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="32" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="19">
         <f>AVERAGE(D8:D11)</f>
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <f>AVERAGE(E8:E11)</f>
         <v>9.8958333333333342E-4</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="19">
         <f t="shared" ref="F12" si="2">AVERAGE(F8:F11)</f>
         <v>2.8182870370370371E-3</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="21">
         <f t="shared" ref="G12" si="3">AVERAGE(G8:G11)</f>
         <v>7.5231481481481482E-4</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="19">
         <f t="shared" ref="H12" si="4">AVERAGE(H8:H11)</f>
         <v>5.8912037037037041E-3</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="21">
         <f t="shared" ref="I12" si="5">AVERAGE(I8:I11)</f>
         <v>7.1180555555555559E-4</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="19">
         <f t="shared" ref="J12" si="6">AVERAGE(J8:J11)</f>
         <v>1.5625000000000001E-3</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="19">
+        <f>SUM(D12:J12)</f>
+        <v>2.0954861111111112E-2</v>
+      </c>
+      <c r="L12" s="43">
         <f t="shared" si="0"/>
-        <v>2.0954861111111112E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="23">
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="24">
         <v>1.7939814814814815E-3</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="23">
         <v>3.0324074074074073E-3</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="25">
         <v>7.7546296296296304E-4</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="23">
         <v>7.2569444444444443E-3</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="25">
         <v>8.3333333333333339E-4</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="23">
         <v>1.9212962962962962E-3</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="23">
+        <f>SUM(D13:J13)</f>
+        <v>2.3842592592592589E-2</v>
+      </c>
+      <c r="L13" s="44">
         <f t="shared" si="0"/>
-        <v>2.3842592592592589E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="23"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="22"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="23">
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="24">
         <v>7.407407407407407E-4</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="23">
         <v>2.8935185185185188E-3</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="25">
         <v>9.4907407407407408E-4</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="23">
         <v>7.3611111111111108E-3</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <v>8.449074074074075E-4</v>
       </c>
-      <c r="J14" s="24">
+      <c r="J14" s="23">
         <v>1.9212962962962962E-3</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="23">
+        <f>SUM(D14:J14)</f>
+        <v>2.2939814814814816E-2</v>
+      </c>
+      <c r="L14" s="44">
         <f t="shared" si="0"/>
-        <v>2.2939814814814816E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24">
+      <c r="C15" s="34"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23">
+        <f>SUM(D15:J15)</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+    <row r="16" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24">
+      <c r="C16" s="34"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23">
+        <f>SUM(D16:J16)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
+    <row r="17" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="26" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="27">
         <f>AVERAGE(D13:D16)</f>
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="28">
         <f>AVERAGE(E13:E16)</f>
         <v>1.267361111111111E-3</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="27">
         <f t="shared" ref="F17" si="7">AVERAGE(F13:F16)</f>
         <v>2.9629629629629632E-3</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="29">
         <f t="shared" ref="G17" si="8">AVERAGE(G13:G16)</f>
         <v>8.6226851851851851E-4</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="27">
         <f t="shared" ref="H17" si="9">AVERAGE(H13:H16)</f>
         <v>7.3090277777777771E-3</v>
       </c>
-      <c r="I17" s="30">
+      <c r="I17" s="29">
         <f t="shared" ref="I17" si="10">AVERAGE(I13:I16)</f>
         <v>8.391203703703705E-4</v>
       </c>
-      <c r="J17" s="28">
+      <c r="J17" s="27">
         <f t="shared" ref="J17" si="11">AVERAGE(J13:J16)</f>
         <v>1.9212962962962962E-3</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17" s="27">
+        <f>SUM(D17:J17)</f>
+        <v>2.3391203703703706E-2</v>
+      </c>
+      <c r="L17" s="45">
         <f t="shared" si="0"/>
-        <v>2.3391203703703706E-2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revet to m4.xlarge instances
</commit_message>
<xml_diff>
--- a/asystem-adoc/src/site/resources/altus_spark_sizing.xlsx
+++ b/asystem-adoc/src/site/resources/altus_spark_sizing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graham/_/dev/graham/asystem/asystem-adoc/src/site/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE14DC8-B29A-294D-A49C-1BC62494D8B8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E70E90C-EB49-B042-8CBF-68AFB0181E1C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5060" yWindow="2900" windowWidth="43300" windowHeight="20200" xr2:uid="{342B7839-8DF3-8649-8032-CC038C3B89CC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>export CLUSTER_INSTANCE_TYPE=c4.xlarge</t>
   </si>
@@ -69,9 +69,6 @@
     <t xml:space="preserve"> intraday-training</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
     <t>provision</t>
   </si>
   <si>
@@ -82,6 +79,18 @@
   </si>
   <si>
     <t>export SPARK_EXEC_MEMORY=1400m</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>unit cost</t>
+  </si>
+  <si>
+    <t>total cost</t>
+  </si>
+  <si>
+    <t>nodes</t>
   </si>
 </sst>
 </file>
@@ -256,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -273,9 +282,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -285,66 +291,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="45" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -369,12 +321,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -397,6 +343,90 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -713,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97B9F99-D795-2747-B80E-3F5C45A90888}">
-  <dimension ref="B1:L17"/>
+  <dimension ref="B1:N17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,494 +754,590 @@
     <col min="1" max="1" width="4.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="38.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="10" style="4" customWidth="1"/>
-    <col min="4" max="12" width="19.5" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="4"/>
+    <col min="4" max="14" width="18.6640625" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+    <row r="1" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="10">
+        <v>21</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="32">
         <v>8.0555555555555554E-3</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="33">
         <v>8.2175925925925917E-4</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="32">
         <v>2.9166666666666668E-3</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="34">
         <v>9.0277777777777784E-4</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="32">
         <v>7.9976851851851858E-3</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="34">
         <v>9.7222222222222209E-4</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="32">
         <v>-1</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="32">
         <f>SUM(D3:J3)</f>
         <v>-0.97833333333333328</v>
       </c>
-      <c r="L3" s="40">
-        <f>IF(K3&lt;0,0,ROUND(K3,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10">
+      <c r="L3" s="49">
+        <v>3</v>
+      </c>
+      <c r="M3" s="19">
+        <v>0.19</v>
+      </c>
+      <c r="N3" s="19">
+        <f t="shared" ref="N3:N7" si="0">IF(K3&gt;0,ROUNDUP(K3*24,0)*M3*L3,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="8"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32">
         <f>SUM(D4:J4)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="40">
-        <f t="shared" ref="L4:L17" si="0">IF(K4&lt;0,0,ROUND(K4,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="9" t="s">
+      <c r="L4" s="49">
+        <v>3</v>
+      </c>
+      <c r="M4" s="19">
+        <v>0.19</v>
+      </c>
+      <c r="N4" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10">
+      <c r="C5" s="29"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32">
         <f>SUM(D5:J5)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="40">
+      <c r="L5" s="49">
+        <v>3</v>
+      </c>
+      <c r="M5" s="19">
+        <v>0.19</v>
+      </c>
+      <c r="N5" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10">
+      <c r="C6" s="30"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32">
         <f>SUM(D6:J6)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="40">
+      <c r="L6" s="49">
+        <v>3</v>
+      </c>
+      <c r="M6" s="19">
+        <v>0.19</v>
+      </c>
+      <c r="N6" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="47" t="s">
-        <v>18</v>
+    <row r="7" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="26" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="13">
+        <v>16</v>
+      </c>
+      <c r="D7" s="35">
         <f>AVERAGE(D3:D6)</f>
         <v>8.0555555555555554E-3</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="36">
         <f>AVERAGE(E3:E6)</f>
         <v>8.2175925925925917E-4</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="35">
         <f t="shared" ref="F7:J7" si="1">AVERAGE(F3:F6)</f>
         <v>2.9166666666666668E-3</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="37">
         <f t="shared" si="1"/>
         <v>9.0277777777777784E-4</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="35">
         <f t="shared" si="1"/>
         <v>7.9976851851851858E-3</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="37">
         <f t="shared" si="1"/>
         <v>9.7222222222222209E-4</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="35">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="35">
         <f>SUM(D7:J7)</f>
         <v>-0.97833333333333328</v>
       </c>
-      <c r="L7" s="41">
+      <c r="L7" s="50">
+        <v>3</v>
+      </c>
+      <c r="M7" s="20">
+        <v>0.19</v>
+      </c>
+      <c r="N7" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="16">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="31">
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="38">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="31">
         <v>3.1365740740740742E-3</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="39">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="31">
         <v>5.7060185185185191E-3</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="39">
         <v>7.291666666666667E-4</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="31">
         <v>1.6087962962962963E-3</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="31">
         <f>SUM(D8:J8)</f>
         <v>2.0798611111111108E-2</v>
       </c>
-      <c r="L8" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="31"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="16">
+      <c r="L8" s="51">
+        <v>3</v>
+      </c>
+      <c r="M8" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="N8" s="21">
+        <f>IF(K8&gt;0,ROUNDUP(K8*24,0)*M8*L8,0)</f>
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B9" s="12"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="31">
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="38">
         <v>1.2847222222222223E-3</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="31">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="39">
         <v>8.1018518518518516E-4</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="31">
         <v>6.076388888888889E-3</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="39">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="31">
         <v>1.5162037037037036E-3</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="31">
         <f>SUM(D9:J9)</f>
         <v>2.1111111111111112E-2</v>
       </c>
-      <c r="L9" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="31" t="s">
+      <c r="L9" s="51">
+        <v>3</v>
+      </c>
+      <c r="M9" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="N9" s="21">
+        <f t="shared" ref="N9:N17" si="2">IF(K9&gt;0,ROUNDUP(K9*24,0)*M9*L9,0)</f>
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16">
+      <c r="C10" s="17"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31">
         <f>SUM(D10:J10)</f>
         <v>0</v>
       </c>
-      <c r="L10" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
+      <c r="L10" s="51">
+        <v>3</v>
+      </c>
+      <c r="M10" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="N10" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16">
+      <c r="C11" s="18"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31">
         <f>SUM(D11:J11)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="32" t="s">
+      <c r="L11" s="51">
+        <v>3</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="N11" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="19">
+        <v>16</v>
+      </c>
+      <c r="D12" s="40">
         <f>AVERAGE(D8:D11)</f>
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="41">
         <f>AVERAGE(E8:E11)</f>
         <v>9.8958333333333342E-4</v>
       </c>
-      <c r="F12" s="19">
-        <f t="shared" ref="F12" si="2">AVERAGE(F8:F11)</f>
+      <c r="F12" s="40">
+        <f t="shared" ref="F12" si="3">AVERAGE(F8:F11)</f>
         <v>2.8182870370370371E-3</v>
       </c>
-      <c r="G12" s="21">
-        <f t="shared" ref="G12" si="3">AVERAGE(G8:G11)</f>
+      <c r="G12" s="42">
+        <f t="shared" ref="G12" si="4">AVERAGE(G8:G11)</f>
         <v>7.5231481481481482E-4</v>
       </c>
-      <c r="H12" s="19">
-        <f t="shared" ref="H12" si="4">AVERAGE(H8:H11)</f>
+      <c r="H12" s="40">
+        <f t="shared" ref="H12" si="5">AVERAGE(H8:H11)</f>
         <v>5.8912037037037041E-3</v>
       </c>
-      <c r="I12" s="21">
-        <f t="shared" ref="I12" si="5">AVERAGE(I8:I11)</f>
+      <c r="I12" s="42">
+        <f t="shared" ref="I12" si="6">AVERAGE(I8:I11)</f>
         <v>7.1180555555555559E-4</v>
       </c>
-      <c r="J12" s="19">
-        <f t="shared" ref="J12" si="6">AVERAGE(J8:J11)</f>
+      <c r="J12" s="40">
+        <f t="shared" ref="J12" si="7">AVERAGE(J8:J11)</f>
         <v>1.5625000000000001E-3</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="40">
         <f>SUM(D12:J12)</f>
         <v>2.0954861111111112E-2</v>
       </c>
-      <c r="L12" s="43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="23">
+      <c r="L12" s="52">
+        <v>3</v>
+      </c>
+      <c r="M12" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="N12" s="22">
+        <f t="shared" si="2"/>
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="43">
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="44">
         <v>1.7939814814814815E-3</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="43">
         <v>3.0324074074074073E-3</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="45">
         <v>7.7546296296296304E-4</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="43">
         <v>7.2569444444444443E-3</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="45">
         <v>8.3333333333333339E-4</v>
       </c>
-      <c r="J13" s="23">
+      <c r="J13" s="43">
         <v>1.9212962962962962E-3</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="43">
         <f>SUM(D13:J13)</f>
         <v>2.3842592592592589E-2</v>
       </c>
-      <c r="L13" s="44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="22"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="23">
+      <c r="L13" s="53">
+        <v>3</v>
+      </c>
+      <c r="M13" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="N13" s="23">
+        <f t="shared" si="2"/>
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="9"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="43">
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="44">
         <v>7.407407407407407E-4</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="43">
         <v>2.8935185185185188E-3</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="45">
         <v>9.4907407407407408E-4</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="43">
         <v>7.3611111111111108E-3</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="45">
         <v>8.449074074074075E-4</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="43">
         <v>1.9212962962962962E-3</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="43">
         <f>SUM(D14:J14)</f>
         <v>2.2939814814814816E-2</v>
       </c>
-      <c r="L14" s="44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="22" t="s">
+      <c r="L14" s="53">
+        <v>3</v>
+      </c>
+      <c r="M14" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="N14" s="23">
+        <f t="shared" si="2"/>
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23">
+      <c r="C15" s="15"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43">
         <f>SUM(D15:J15)</f>
         <v>0</v>
       </c>
-      <c r="L15" s="44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="s">
+      <c r="L15" s="53">
+        <v>3</v>
+      </c>
+      <c r="M15" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="N15" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23">
+      <c r="C16" s="15"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43">
         <f>SUM(D16:J16)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="26" t="s">
+      <c r="L16" s="53">
+        <v>3</v>
+      </c>
+      <c r="M16" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="N16" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="27">
+        <v>16</v>
+      </c>
+      <c r="D17" s="46">
         <f>AVERAGE(D13:D16)</f>
         <v>8.2291666666666659E-3</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="47">
         <f>AVERAGE(E13:E16)</f>
         <v>1.267361111111111E-3</v>
       </c>
-      <c r="F17" s="27">
-        <f t="shared" ref="F17" si="7">AVERAGE(F13:F16)</f>
+      <c r="F17" s="46">
+        <f t="shared" ref="F17" si="8">AVERAGE(F13:F16)</f>
         <v>2.9629629629629632E-3</v>
       </c>
-      <c r="G17" s="29">
-        <f t="shared" ref="G17" si="8">AVERAGE(G13:G16)</f>
+      <c r="G17" s="48">
+        <f t="shared" ref="G17" si="9">AVERAGE(G13:G16)</f>
         <v>8.6226851851851851E-4</v>
       </c>
-      <c r="H17" s="27">
-        <f t="shared" ref="H17" si="9">AVERAGE(H13:H16)</f>
+      <c r="H17" s="46">
+        <f t="shared" ref="H17" si="10">AVERAGE(H13:H16)</f>
         <v>7.3090277777777771E-3</v>
       </c>
-      <c r="I17" s="29">
-        <f t="shared" ref="I17" si="10">AVERAGE(I13:I16)</f>
+      <c r="I17" s="48">
+        <f t="shared" ref="I17" si="11">AVERAGE(I13:I16)</f>
         <v>8.391203703703705E-4</v>
       </c>
-      <c r="J17" s="27">
-        <f t="shared" ref="J17" si="11">AVERAGE(J13:J16)</f>
+      <c r="J17" s="46">
+        <f t="shared" ref="J17" si="12">AVERAGE(J13:J16)</f>
         <v>1.9212962962962962E-3</v>
       </c>
-      <c r="K17" s="27">
+      <c r="K17" s="46">
         <f>SUM(D17:J17)</f>
         <v>2.3391203703703706E-2</v>
       </c>
-      <c r="L17" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="L17" s="54">
+        <v>3</v>
+      </c>
+      <c r="M17" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="N17" s="24">
+        <f t="shared" si="2"/>
+        <v>0.60000000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert altus instance and spark sizing
</commit_message>
<xml_diff>
--- a/asystem-adoc/src/site/resources/altus_spark_sizing.xlsx
+++ b/asystem-adoc/src/site/resources/altus_spark_sizing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graham/_/dev/graham/asystem/asystem-adoc/src/site/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C19D9D-B396-C04A-B3DB-D6AABDCABB76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D301E60-66A8-AD44-83C6-4508ACA24CBC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5060" yWindow="2900" windowWidth="43300" windowHeight="20200" xr2:uid="{342B7839-8DF3-8649-8032-CC038C3B89CC}"/>
+    <workbookView xWindow="3160" yWindow="3600" windowWidth="43600" windowHeight="18160" xr2:uid="{342B7839-8DF3-8649-8032-CC038C3B89CC}"/>
   </bookViews>
   <sheets>
     <sheet name="10.000.0080" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>export CLUSTER_INSTANCE_TYPE=c4.xlarge</t>
   </si>
@@ -78,9 +78,6 @@
     <t>export SPARK_EXEC_MEMORY=1400m</t>
   </si>
   <si>
-    <t>minutes</t>
-  </si>
-  <si>
     <t>unit cost</t>
   </si>
   <si>
@@ -100,6 +97,15 @@
   </si>
   <si>
     <t>export SPARK_EXEC_MEMORY=4000m</t>
+  </si>
+  <si>
+    <t>export SPARK_EXEC_NUM=5</t>
+  </si>
+  <si>
+    <t>destroy</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -300,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -513,12 +519,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -841,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97B9F99-D795-2747-B80E-3F5C45A90888}">
-  <dimension ref="B1:N22"/>
+  <dimension ref="B1:O22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,12 +852,12 @@
     <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="14" width="18.6640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="15" width="18.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
@@ -882,19 +882,22 @@
         <v>13</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -923,24 +926,27 @@
         <v>-1</v>
       </c>
       <c r="K3" s="8">
-        <f>SUM(D3:J3)</f>
-        <v>-0.97833333333333328</v>
-      </c>
-      <c r="L3" s="11" t="str">
-        <f>RIGHT($B$6, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="M3" s="12">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L3" s="8">
+        <f>D3+SUM(E3:G3)*2+SUM(H3:K3)</f>
+        <v>-0.97021990740740738</v>
+      </c>
+      <c r="M3" s="11" t="str">
+        <f>RIGHT($B$4, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="N3" s="12">
         <v>0.19</v>
       </c>
-      <c r="N3" s="12">
-        <f>IF(K3&gt;0,ROUNDUP(K3*24,0)*M3*L3,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O3" s="12" t="str">
+        <f>IF(L3&gt;0,ROUNDUP(L3*24,0)*N3*M3,"###################")</f>
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="8"/>
@@ -950,23 +956,24 @@
       <c r="H4" s="8"/>
       <c r="I4" s="10"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="8">
-        <f>SUM(D4:J4)</f>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8">
+        <f t="shared" ref="L4:L22" si="0">D4+SUM(E4:G4)*2+SUM(H4:K4)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="11" t="str">
-        <f t="shared" ref="L4:L7" si="0">RIGHT($B$6, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11" t="str">
+        <f t="shared" ref="M4:M6" si="1">RIGHT($B$4, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="N4" s="12">
         <v>0.19</v>
       </c>
-      <c r="N4" s="12">
-        <f t="shared" ref="N3:N12" si="1">IF(K4&gt;0,ROUNDUP(K4*24,0)*M4*L4,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="12" t="str">
+        <f t="shared" ref="O4:O22" si="2">IF(L4&gt;0,ROUNDUP(L4*24,0)*N4*M4,"###################")</f>
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
@@ -978,23 +985,24 @@
       <c r="H5" s="8"/>
       <c r="I5" s="10"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="8">
-        <f>SUM(D5:J5)</f>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M5" s="12">
+      <c r="M5" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N5" s="12">
         <v>0.19</v>
       </c>
-      <c r="N5" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>2</v>
       </c>
@@ -1006,28 +1014,29 @@
       <c r="H6" s="8"/>
       <c r="I6" s="10"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="8">
-        <f>SUM(D6:J6)</f>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L6" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M6" s="12">
+      <c r="M6" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N6" s="12">
         <v>0.19</v>
       </c>
-      <c r="N6" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="18">
         <f>AVERAGE(D3:D6)</f>
@@ -1038,96 +1047,140 @@
         <v>8.2175925925925917E-4</v>
       </c>
       <c r="F7" s="18">
-        <f t="shared" ref="F7:J7" si="2">AVERAGE(F3:F6)</f>
+        <f t="shared" ref="F7:J7" si="3">AVERAGE(F3:F6)</f>
         <v>2.9166666666666668E-3</v>
       </c>
       <c r="G7" s="20">
+        <f t="shared" si="3"/>
+        <v>9.0277777777777784E-4</v>
+      </c>
+      <c r="H7" s="18">
+        <f t="shared" si="3"/>
+        <v>7.9976851851851858E-3</v>
+      </c>
+      <c r="I7" s="20">
+        <f t="shared" si="3"/>
+        <v>9.7222222222222209E-4</v>
+      </c>
+      <c r="J7" s="18">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="K7" s="18">
+        <f>AVERAGE(K3:K6)</f>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L7" s="18">
+        <f t="shared" si="0"/>
+        <v>-0.97021990740740738</v>
+      </c>
+      <c r="M7" s="21" t="str">
+        <f>RIGHT($B$4, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="N7" s="22">
+        <v>0.19</v>
+      </c>
+      <c r="O7" s="22" t="str">
         <f t="shared" si="2"/>
-        <v>9.0277777777777784E-4</v>
-      </c>
-      <c r="H7" s="18">
-        <f t="shared" si="2"/>
-        <v>7.9976851851851858E-3</v>
-      </c>
-      <c r="I7" s="20">
-        <f t="shared" si="2"/>
-        <v>9.7222222222222209E-4</v>
-      </c>
-      <c r="J7" s="18">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="K7" s="18">
-        <f>SUM(D7:J7)</f>
-        <v>-0.97833333333333328</v>
-      </c>
-      <c r="L7" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M7" s="22">
-        <v>0.19</v>
-      </c>
-      <c r="N7" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="65" t="str">
-        <f>RIGHT($B$11, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="M8" s="66">
+      <c r="D8" s="62">
+        <v>8.0555555555555554E-3</v>
+      </c>
+      <c r="E8" s="62">
+        <v>7.5231481481481471E-4</v>
+      </c>
+      <c r="F8" s="63">
+        <v>2.3263888888888887E-3</v>
+      </c>
+      <c r="G8" s="64">
+        <v>5.6712962962962956E-4</v>
+      </c>
+      <c r="H8" s="63">
+        <v>3.9120370370370368E-3</v>
+      </c>
+      <c r="I8" s="64">
+        <v>9.2592592592592585E-4</v>
+      </c>
+      <c r="J8" s="63">
+        <v>1.423611111111111E-3</v>
+      </c>
+      <c r="K8" s="63">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L8" s="63">
+        <f t="shared" si="0"/>
+        <v>2.5081018518518516E-2</v>
+      </c>
+      <c r="M8" s="65" t="str">
+        <f>RIGHT($B$9, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="N8" s="66">
         <v>0.39800000000000002</v>
       </c>
-      <c r="N8" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="66">
+        <f t="shared" si="2"/>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="67" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="68"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="65" t="str">
-        <f t="shared" ref="L9:L12" si="3">RIGHT($B$11, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="M9" s="66">
+      <c r="D9" s="62">
+        <v>8.0555555555555554E-3</v>
+      </c>
+      <c r="E9" s="62">
+        <v>1.1921296296296296E-3</v>
+      </c>
+      <c r="F9" s="63">
+        <v>2.3495370370370371E-3</v>
+      </c>
+      <c r="G9" s="64">
+        <v>8.9120370370370362E-4</v>
+      </c>
+      <c r="H9" s="63">
+        <v>3.7268518518518514E-3</v>
+      </c>
+      <c r="I9" s="64">
+        <v>6.5972222222222213E-4</v>
+      </c>
+      <c r="J9" s="63">
+        <v>1.423611111111111E-3</v>
+      </c>
+      <c r="K9" s="63">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L9" s="63">
+        <f t="shared" si="0"/>
+        <v>2.6203703703703701E-2</v>
+      </c>
+      <c r="M9" s="65" t="str">
+        <f t="shared" ref="M9:M12" si="4">RIGHT($B$9, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="N9" s="66">
         <v>0.39800000000000002</v>
       </c>
-      <c r="N9" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="66">
+        <f t="shared" si="2"/>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="67" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C10" s="68"/>
       <c r="D10" s="62"/>
@@ -1138,19 +1191,23 @@
       <c r="I10" s="64"/>
       <c r="J10" s="63"/>
       <c r="K10" s="63"/>
-      <c r="L10" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="M10" s="66">
+      <c r="L10" s="63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="N10" s="66">
         <v>0.39800000000000002</v>
       </c>
-      <c r="N10" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="66" t="str">
+        <f t="shared" si="2"/>
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="67" t="s">
         <v>2</v>
       </c>
@@ -1163,46 +1220,78 @@
       <c r="I11" s="64"/>
       <c r="J11" s="63"/>
       <c r="K11" s="63"/>
-      <c r="L11" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="M11" s="66">
+      <c r="L11" s="63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="N11" s="66">
         <v>0.39800000000000002</v>
       </c>
-      <c r="N11" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="66" t="str">
+        <f t="shared" si="2"/>
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="69" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="70" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="74" t="str">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="M12" s="75">
+        <v>22</v>
+      </c>
+      <c r="D12" s="71">
+        <f>AVERAGE(D8:D11)</f>
+        <v>8.0555555555555554E-3</v>
+      </c>
+      <c r="E12" s="71">
+        <f t="shared" ref="E12:K12" si="5">AVERAGE(E8:E11)</f>
+        <v>9.7222222222222219E-4</v>
+      </c>
+      <c r="F12" s="71">
+        <f t="shared" si="5"/>
+        <v>2.3379629629629627E-3</v>
+      </c>
+      <c r="G12" s="71">
+        <f t="shared" si="5"/>
+        <v>7.2916666666666659E-4</v>
+      </c>
+      <c r="H12" s="71">
+        <f t="shared" si="5"/>
+        <v>3.8194444444444439E-3</v>
+      </c>
+      <c r="I12" s="71">
+        <f t="shared" si="5"/>
+        <v>7.9282407407407405E-4</v>
+      </c>
+      <c r="J12" s="71">
+        <f t="shared" si="5"/>
+        <v>1.423611111111111E-3</v>
+      </c>
+      <c r="K12" s="71">
+        <f t="shared" si="5"/>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L12" s="71">
+        <f t="shared" si="0"/>
+        <v>2.5642361111111109E-2</v>
+      </c>
+      <c r="M12" s="72" t="str">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="N12" s="73">
         <v>0.39800000000000002</v>
       </c>
-      <c r="N12" s="75">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="73">
+        <f t="shared" si="2"/>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
         <v>3</v>
       </c>
@@ -1231,24 +1320,27 @@
         <v>1.6087962962962963E-3</v>
       </c>
       <c r="K13" s="25">
-        <f t="shared" ref="K13:K22" si="4">SUM(D13:J13)</f>
-        <v>2.0798611111111108E-2</v>
-      </c>
-      <c r="L13" s="28" t="str">
-        <f>RIGHT($B$16, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="M13" s="29">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L13" s="25">
+        <f t="shared" si="0"/>
+        <v>2.8796296296296292E-2</v>
+      </c>
+      <c r="M13" s="28" t="str">
+        <f>RIGHT($B$14, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="N13" s="29">
         <v>0.2</v>
       </c>
-      <c r="N13" s="29">
-        <f>IF(K13&gt;0,ROUNDUP(K13*24,0)*M13*L13,0)</f>
+      <c r="O13" s="29">
+        <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="32">
@@ -1273,22 +1365,25 @@
         <v>1.5162037037037036E-3</v>
       </c>
       <c r="K14" s="32">
-        <f t="shared" si="4"/>
-        <v>2.1111111111111112E-2</v>
-      </c>
-      <c r="L14" s="35" t="str">
-        <f t="shared" ref="L14:L17" si="5">RIGHT($B$16, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="M14" s="36">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L14" s="32">
+        <f t="shared" si="0"/>
+        <v>2.9178240740740741E-2</v>
+      </c>
+      <c r="M14" s="35" t="str">
+        <f t="shared" ref="M14:M17" si="6">RIGHT($B$14, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="N14" s="36">
         <v>0.2</v>
       </c>
-      <c r="N14" s="36">
-        <f t="shared" ref="N14:N22" si="6">IF(K14&gt;0,ROUNDUP(K14*24,0)*M14*L14,0)</f>
+      <c r="O14" s="36">
+        <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="30" t="s">
         <v>1</v>
       </c>
@@ -1300,23 +1395,24 @@
       <c r="H15" s="32"/>
       <c r="I15" s="34"/>
       <c r="J15" s="32"/>
-      <c r="K15" s="32">
-        <f t="shared" si="4"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="M15" s="36">
+      <c r="M15" s="35" t="str">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="N15" s="36">
         <v>0.2</v>
       </c>
-      <c r="N15" s="36">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="30" t="s">
         <v>2</v>
       </c>
@@ -1328,28 +1424,29 @@
       <c r="H16" s="32"/>
       <c r="I16" s="34"/>
       <c r="J16" s="32"/>
-      <c r="K16" s="32">
-        <f t="shared" si="4"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L16" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="M16" s="36">
+      <c r="M16" s="35" t="str">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="N16" s="36">
         <v>0.2</v>
       </c>
-      <c r="N16" s="36">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O16" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="40">
         <f>AVERAGE(D13:D16)</f>
@@ -1376,26 +1473,30 @@
         <v>7.1180555555555559E-4</v>
       </c>
       <c r="J17" s="40">
-        <f t="shared" ref="J17" si="11">AVERAGE(J13:J16)</f>
+        <f t="shared" ref="J17:K17" si="11">AVERAGE(J13:J16)</f>
         <v>1.5625000000000001E-3</v>
       </c>
       <c r="K17" s="40">
-        <f t="shared" si="4"/>
-        <v>2.0954861111111112E-2</v>
-      </c>
-      <c r="L17" s="43" t="str">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="M17" s="44">
+        <f t="shared" si="11"/>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L17" s="40">
+        <f t="shared" si="0"/>
+        <v>2.898726851851852E-2</v>
+      </c>
+      <c r="M17" s="43" t="str">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="N17" s="44">
         <v>0.2</v>
       </c>
-      <c r="N17" s="44">
-        <f t="shared" si="6"/>
+      <c r="O17" s="44">
+        <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="45" t="s">
         <v>3</v>
       </c>
@@ -1424,24 +1525,27 @@
         <v>1.9212962962962962E-3</v>
       </c>
       <c r="K18" s="47">
-        <f t="shared" si="4"/>
-        <v>2.3842592592592589E-2</v>
-      </c>
-      <c r="L18" s="50" t="str">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L18" s="47">
+        <f t="shared" si="0"/>
+        <v>3.2916666666666664E-2</v>
+      </c>
+      <c r="M18" s="50" t="str">
         <f>RIGHT($B$19, 1)</f>
         <v>3</v>
       </c>
-      <c r="M18" s="51">
+      <c r="N18" s="51">
         <v>0.2</v>
       </c>
-      <c r="N18" s="51">
-        <f t="shared" si="6"/>
+      <c r="O18" s="51">
+        <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="52"/>
       <c r="D19" s="47">
@@ -1466,22 +1570,25 @@
         <v>1.9212962962962962E-3</v>
       </c>
       <c r="K19" s="47">
-        <f t="shared" si="4"/>
-        <v>2.2939814814814816E-2</v>
-      </c>
-      <c r="L19" s="50" t="str">
-        <f t="shared" ref="L19:L22" si="12">RIGHT($B$19, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="M19" s="51">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L19" s="47">
+        <f t="shared" si="0"/>
+        <v>3.0995370370370368E-2</v>
+      </c>
+      <c r="M19" s="50" t="str">
+        <f t="shared" ref="M19:M22" si="12">RIGHT($B$19, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="N19" s="51">
         <v>0.2</v>
       </c>
-      <c r="N19" s="51">
-        <f t="shared" si="6"/>
+      <c r="O19" s="51">
+        <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="45" t="s">
         <v>4</v>
       </c>
@@ -1493,23 +1600,24 @@
       <c r="H20" s="47"/>
       <c r="I20" s="49"/>
       <c r="J20" s="47"/>
-      <c r="K20" s="47">
-        <f t="shared" si="4"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L20" s="50" t="str">
+      <c r="M20" s="50" t="str">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="M20" s="51">
+      <c r="N20" s="51">
         <v>0.2</v>
       </c>
-      <c r="N20" s="51">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O20" s="51" t="str">
+        <f t="shared" si="2"/>
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="45" t="s">
         <v>5</v>
       </c>
@@ -1521,28 +1629,29 @@
       <c r="H21" s="47"/>
       <c r="I21" s="49"/>
       <c r="J21" s="47"/>
-      <c r="K21" s="47">
-        <f t="shared" si="4"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L21" s="50" t="str">
+      <c r="M21" s="50" t="str">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="M21" s="51">
+      <c r="N21" s="51">
         <v>0.2</v>
       </c>
-      <c r="N21" s="51">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O21" s="51" t="str">
+        <f t="shared" si="2"/>
+        <v>###################</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="53" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="55">
         <f>AVERAGE(D18:D21)</f>
@@ -1569,22 +1678,26 @@
         <v>8.391203703703705E-4</v>
       </c>
       <c r="J22" s="55">
-        <f t="shared" ref="J22" si="17">AVERAGE(J18:J21)</f>
+        <f t="shared" ref="J22:K22" si="17">AVERAGE(J18:J21)</f>
         <v>1.9212962962962962E-3</v>
       </c>
       <c r="K22" s="55">
-        <f t="shared" si="4"/>
-        <v>2.3391203703703706E-2</v>
-      </c>
-      <c r="L22" s="58" t="str">
+        <f t="shared" si="17"/>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L22" s="55">
+        <f t="shared" si="0"/>
+        <v>3.1956018518518516E-2</v>
+      </c>
+      <c r="M22" s="58" t="str">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="M22" s="59">
+      <c r="N22" s="59">
         <v>0.2</v>
       </c>
-      <c r="N22" s="59">
-        <f t="shared" si="6"/>
+      <c r="O22" s="59">
+        <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
       </c>
     </row>

</xml_diff>